<commit_message>
Finished cvtdb to template conversion logic
</commit_message>
<xml_diff>
--- a/input/template_map.xlsx
+++ b/input/template_map.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Lab\HEM\T_Wall_Projects_FY20\cvtdb\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F248FBD-AACF-4F57-AFBC-27607A26ECC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F10722-D849-459F-B5FB-B2F2A9C67AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3324" windowWidth="17280" windowHeight="8964" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
+    <workbookView xWindow="4788" yWindow="996" windowWidth="17280" windowHeight="8964" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$85</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="101">
   <si>
     <t>from</t>
   </si>
@@ -316,6 +316,30 @@
   </si>
   <si>
     <t>administration_term</t>
+  </si>
+  <si>
+    <t>test_substance_name_secondary_original</t>
+  </si>
+  <si>
+    <t>test_substance_casrn_original</t>
+  </si>
+  <si>
+    <t>dose_volume_units</t>
+  </si>
+  <si>
+    <t>extracted</t>
+  </si>
+  <si>
+    <t>document_type</t>
+  </si>
+  <si>
+    <t>fk_reference_document_id</t>
+  </si>
+  <si>
+    <t>conc_cumulative</t>
+  </si>
+  <si>
+    <t>clowder_file_id</t>
   </si>
 </sst>
 </file>
@@ -667,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1B38F2-9BC7-48A6-ACF9-07AB94F89F72}">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,10 +720,10 @@
         <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -707,10 +731,10 @@
         <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -718,10 +742,10 @@
         <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -729,10 +753,10 @@
         <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -740,10 +764,10 @@
         <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -751,10 +775,10 @@
         <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -762,10 +786,10 @@
         <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -773,54 +797,54 @@
         <v>86</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -828,10 +852,10 @@
         <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -839,10 +863,10 @@
         <v>87</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -850,10 +874,10 @@
         <v>87</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -861,10 +885,10 @@
         <v>87</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -872,10 +896,10 @@
         <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -883,10 +907,10 @@
         <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -894,10 +918,10 @@
         <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -905,10 +929,10 @@
         <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -916,10 +940,10 @@
         <v>87</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -927,10 +951,10 @@
         <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -938,10 +962,10 @@
         <v>87</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -949,10 +973,10 @@
         <v>87</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -960,10 +984,10 @@
         <v>87</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -971,10 +995,10 @@
         <v>87</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C27" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -982,10 +1006,10 @@
         <v>87</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="C28" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -993,10 +1017,10 @@
         <v>87</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1004,10 +1028,10 @@
         <v>87</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1015,10 +1039,10 @@
         <v>87</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1026,10 +1050,10 @@
         <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -1037,10 +1061,10 @@
         <v>87</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1048,76 +1072,76 @@
         <v>87</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C40" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1125,10 +1149,10 @@
         <v>88</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1136,10 +1160,10 @@
         <v>88</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C42" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1147,10 +1171,10 @@
         <v>88</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1158,10 +1182,10 @@
         <v>88</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C44" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1169,10 +1193,10 @@
         <v>88</v>
       </c>
       <c r="B45" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C45" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1180,76 +1204,76 @@
         <v>88</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="C46" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B48" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="C48" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B49" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C49" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C50" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B51" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C51" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B52" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="C52" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -1257,10 +1281,10 @@
         <v>89</v>
       </c>
       <c r="B53" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="C53" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -1268,10 +1292,10 @@
         <v>89</v>
       </c>
       <c r="B54" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="C54" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1279,10 +1303,10 @@
         <v>89</v>
       </c>
       <c r="B55" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C55" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1290,10 +1314,10 @@
         <v>89</v>
       </c>
       <c r="B56" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C56" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -1301,10 +1325,10 @@
         <v>89</v>
       </c>
       <c r="B57" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C57" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1312,10 +1336,10 @@
         <v>89</v>
       </c>
       <c r="B58" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="C58" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -1323,10 +1347,10 @@
         <v>89</v>
       </c>
       <c r="B59" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="C59" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1334,10 +1358,10 @@
         <v>89</v>
       </c>
       <c r="B60" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="C60" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -1345,10 +1369,10 @@
         <v>89</v>
       </c>
       <c r="B61" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C61" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -1356,10 +1380,10 @@
         <v>89</v>
       </c>
       <c r="B62" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C62" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -1367,10 +1391,10 @@
         <v>89</v>
       </c>
       <c r="B63" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C63" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1378,10 +1402,10 @@
         <v>89</v>
       </c>
       <c r="B64" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="C64" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1389,10 +1413,10 @@
         <v>89</v>
       </c>
       <c r="B65" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C65" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1400,10 +1424,10 @@
         <v>89</v>
       </c>
       <c r="B66" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="C66" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -1411,10 +1435,10 @@
         <v>89</v>
       </c>
       <c r="B67" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="C67" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -1422,10 +1446,10 @@
         <v>89</v>
       </c>
       <c r="B68" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C68" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -1433,10 +1457,10 @@
         <v>89</v>
       </c>
       <c r="B69" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C69" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -1444,10 +1468,10 @@
         <v>89</v>
       </c>
       <c r="B70" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="C70" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -1455,81 +1479,81 @@
         <v>89</v>
       </c>
       <c r="B71" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="C71" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B72" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C72" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B73" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="C73" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B74" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="C74" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B75" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="C75" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B76" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="C76" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B77" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C77" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B78" t="s">
         <v>9</v>
@@ -1538,8 +1562,85 @@
         <v>9</v>
       </c>
     </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>90</v>
+      </c>
+      <c r="B79" t="s">
+        <v>66</v>
+      </c>
+      <c r="C79" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>90</v>
+      </c>
+      <c r="B80" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>90</v>
+      </c>
+      <c r="B81" t="s">
+        <v>82</v>
+      </c>
+      <c r="C81" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>90</v>
+      </c>
+      <c r="B82" t="s">
+        <v>85</v>
+      </c>
+      <c r="C82" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>90</v>
+      </c>
+      <c r="B83" t="s">
+        <v>83</v>
+      </c>
+      <c r="C83" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>90</v>
+      </c>
+      <c r="B84" t="s">
+        <v>84</v>
+      </c>
+      <c r="C84" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>90</v>
+      </c>
+      <c r="B85" t="s">
+        <v>9</v>
+      </c>
+      <c r="C85" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C78" xr:uid="{461A9C18-F1C7-4A34-90BC-0952E60C20C5}"/>
+  <autoFilter ref="A1:C85" xr:uid="{461A9C18-F1C7-4A34-90BC-0952E60C20C5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
HotFix adding missing QC fields to script output
</commit_message>
<xml_diff>
--- a/input/template_map.xlsx
+++ b/input/template_map.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Lab\HEM\T_Wall_Projects_FY20\cvtdb\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F10722-D849-459F-B5FB-B2F2A9C67AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4788" yWindow="996" windowWidth="17280" windowHeight="8964" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$99</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="105">
   <si>
     <t>from</t>
   </si>
@@ -340,6 +340,18 @@
   </si>
   <si>
     <t>clowder_file_id</t>
+  </si>
+  <si>
+    <t>qc_reviewer_lanid</t>
+  </si>
+  <si>
+    <t>qc_notes</t>
+  </si>
+  <si>
+    <t>qc_status</t>
+  </si>
+  <si>
+    <t>qc_flags</t>
   </si>
 </sst>
 </file>
@@ -691,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1B38F2-9BC7-48A6-ACF9-07AB94F89F72}">
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100:C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -849,46 +861,46 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>101</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C15" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -896,10 +908,10 @@
         <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -907,10 +919,10 @@
         <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -918,10 +930,10 @@
         <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -929,10 +941,10 @@
         <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -940,10 +952,10 @@
         <v>87</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -951,10 +963,10 @@
         <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -962,10 +974,10 @@
         <v>87</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -973,10 +985,10 @@
         <v>87</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -984,10 +996,10 @@
         <v>87</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -995,10 +1007,10 @@
         <v>87</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1006,10 +1018,10 @@
         <v>87</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>95</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1017,10 +1029,10 @@
         <v>87</v>
       </c>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C29" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1028,10 +1040,10 @@
         <v>87</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C30" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1039,10 +1051,10 @@
         <v>87</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1050,10 +1062,10 @@
         <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -1061,10 +1073,10 @@
         <v>87</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C33" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1072,10 +1084,10 @@
         <v>87</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C34" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1083,10 +1095,10 @@
         <v>87</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1094,10 +1106,10 @@
         <v>87</v>
       </c>
       <c r="B36" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1105,10 +1117,10 @@
         <v>87</v>
       </c>
       <c r="B37" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C37" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1116,10 +1128,10 @@
         <v>87</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C38" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1127,10 +1139,10 @@
         <v>87</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C39" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1138,87 +1150,87 @@
         <v>87</v>
       </c>
       <c r="B40" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C40" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B42" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C42" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C43" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C44" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="C45" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B46" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="C46" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="C47" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1226,10 +1238,10 @@
         <v>88</v>
       </c>
       <c r="B48" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1237,10 +1249,10 @@
         <v>88</v>
       </c>
       <c r="B49" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C49" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1248,10 +1260,10 @@
         <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C50" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -1259,10 +1271,10 @@
         <v>88</v>
       </c>
       <c r="B51" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C51" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -1270,120 +1282,120 @@
         <v>88</v>
       </c>
       <c r="B52" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="C52" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B53" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C53" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B54" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="C54" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B55" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C55" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B56" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C56" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B57" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C57" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B58" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C58" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B59" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B60" t="s">
-        <v>49</v>
+        <v>102</v>
       </c>
       <c r="C60" t="s">
-        <v>49</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B61" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="C61" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B62" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="C62" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -1391,10 +1403,10 @@
         <v>89</v>
       </c>
       <c r="B63" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="C63" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1402,10 +1414,10 @@
         <v>89</v>
       </c>
       <c r="B64" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="C64" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1413,10 +1425,10 @@
         <v>89</v>
       </c>
       <c r="B65" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="C65" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1424,10 +1436,10 @@
         <v>89</v>
       </c>
       <c r="B66" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C66" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -1435,10 +1447,10 @@
         <v>89</v>
       </c>
       <c r="B67" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="C67" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -1446,10 +1458,10 @@
         <v>89</v>
       </c>
       <c r="B68" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C68" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -1457,10 +1469,10 @@
         <v>89</v>
       </c>
       <c r="B69" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C69" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -1468,10 +1480,10 @@
         <v>89</v>
       </c>
       <c r="B70" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C70" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -1479,10 +1491,10 @@
         <v>89</v>
       </c>
       <c r="B71" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C71" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -1490,10 +1502,10 @@
         <v>89</v>
       </c>
       <c r="B72" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C72" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -1501,10 +1513,10 @@
         <v>89</v>
       </c>
       <c r="B73" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C73" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
@@ -1512,10 +1524,10 @@
         <v>89</v>
       </c>
       <c r="B74" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="C74" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -1523,10 +1535,10 @@
         <v>89</v>
       </c>
       <c r="B75" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C75" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -1534,10 +1546,10 @@
         <v>89</v>
       </c>
       <c r="B76" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C76" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -1545,10 +1557,10 @@
         <v>89</v>
       </c>
       <c r="B77" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C77" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
@@ -1556,91 +1568,278 @@
         <v>89</v>
       </c>
       <c r="B78" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="C78" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B79" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C79" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B80" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="C80" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B81" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="C81" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B82" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C82" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B83" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="C83" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B84" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="C84" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
+        <v>89</v>
+      </c>
+      <c r="B85" t="s">
+        <v>63</v>
+      </c>
+      <c r="C85" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>89</v>
+      </c>
+      <c r="B86" t="s">
+        <v>64</v>
+      </c>
+      <c r="C86" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>89</v>
+      </c>
+      <c r="B87" t="s">
+        <v>78</v>
+      </c>
+      <c r="C87" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>89</v>
+      </c>
+      <c r="B88" t="s">
+        <v>9</v>
+      </c>
+      <c r="C88" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>89</v>
+      </c>
+      <c r="B89" t="s">
+        <v>102</v>
+      </c>
+      <c r="C89" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>103</v>
+      </c>
+      <c r="C90" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>104</v>
+      </c>
+      <c r="C91" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>90</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B92" t="s">
+        <v>11</v>
+      </c>
+      <c r="C92" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>90</v>
+      </c>
+      <c r="B93" t="s">
+        <v>66</v>
+      </c>
+      <c r="C93" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>90</v>
+      </c>
+      <c r="B94" t="s">
+        <v>81</v>
+      </c>
+      <c r="C94" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>90</v>
+      </c>
+      <c r="B95" t="s">
+        <v>82</v>
+      </c>
+      <c r="C95" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>90</v>
+      </c>
+      <c r="B96" t="s">
+        <v>85</v>
+      </c>
+      <c r="C96" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>90</v>
+      </c>
+      <c r="B97" t="s">
+        <v>83</v>
+      </c>
+      <c r="C97" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>90</v>
+      </c>
+      <c r="B98" t="s">
+        <v>84</v>
+      </c>
+      <c r="C98" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>90</v>
+      </c>
+      <c r="B99" t="s">
         <v>9</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C99" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>90</v>
+      </c>
+      <c r="B100" t="s">
+        <v>102</v>
+      </c>
+      <c r="C100" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>90</v>
+      </c>
+      <c r="B101" t="s">
+        <v>103</v>
+      </c>
+      <c r="C101" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>90</v>
+      </c>
+      <c r="B102" t="s">
+        <v>104</v>
+      </c>
+      <c r="C102" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C85" xr:uid="{461A9C18-F1C7-4A34-90BC-0952E60C20C5}"/>
+  <autoFilter ref="A1:C99" xr:uid="{461A9C18-F1C7-4A34-90BC-0952E60C20C5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Draft script to push QC Template back to CvTdb
</commit_message>
<xml_diff>
--- a/input/template_map.xlsx
+++ b/input/template_map.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Lab\HEM\T_Wall_Projects_FY20\cvtdb\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdb-load/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{39BAA12F-EB69-4CAE-B3C5-031ADA0BC3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBEB1669-CCD8-4711-94FF-86BDCA1A7DF0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
+    <workbookView xWindow="4248" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{B484B36D-1F10-4F8F-8807-A5BC8CB5A2EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$104</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="107">
   <si>
     <t>from</t>
   </si>
@@ -276,9 +276,6 @@
     <t>conc_medium_original</t>
   </si>
   <si>
-    <t>log_units</t>
-  </si>
-  <si>
     <t>time_units_original</t>
   </si>
   <si>
@@ -342,24 +339,41 @@
     <t>clowder_file_id</t>
   </si>
   <si>
+    <t>qc_notes</t>
+  </si>
+  <si>
+    <t>qc_status</t>
+  </si>
+  <si>
+    <t>qc_flags</t>
+  </si>
+  <si>
+    <t>analyte_casrn_original</t>
+  </si>
+  <si>
+    <t>analyte_name_secondary_original</t>
+  </si>
+  <si>
+    <t>log_concentration_values</t>
+  </si>
+  <si>
     <t>qc_reviewer_lanid</t>
-  </si>
-  <si>
-    <t>qc_notes</t>
-  </si>
-  <si>
-    <t>qc_status</t>
-  </si>
-  <si>
-    <t>qc_flags</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -387,8 +401,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,534 +718,534 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1B38F2-9BC7-48A6-ACF9-07AB94F89F72}">
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100:C102"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B15" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C15" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="C30" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="C31" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="C34" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="C35" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B36" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="C36" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B38" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C38" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C40" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B41" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="C41" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C42" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B44" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C44" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B45" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="C45" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
       <c r="C46" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B47" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C47" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1238,10 +1253,10 @@
         <v>88</v>
       </c>
       <c r="B48" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1249,10 +1264,10 @@
         <v>88</v>
       </c>
       <c r="B49" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="C49" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1260,10 +1275,10 @@
         <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="C50" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -1271,10 +1286,10 @@
         <v>88</v>
       </c>
       <c r="B51" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="C51" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -1282,10 +1297,10 @@
         <v>88</v>
       </c>
       <c r="B52" t="s">
-        <v>36</v>
+        <v>100</v>
       </c>
       <c r="C52" t="s">
-        <v>36</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -1293,10 +1308,10 @@
         <v>88</v>
       </c>
       <c r="B53" t="s">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="C53" t="s">
-        <v>37</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -1304,10 +1319,10 @@
         <v>88</v>
       </c>
       <c r="B54" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="C54" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1315,10 +1330,10 @@
         <v>88</v>
       </c>
       <c r="B55" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="C55" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1326,10 +1341,10 @@
         <v>88</v>
       </c>
       <c r="B56" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C56" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -1337,10 +1352,10 @@
         <v>88</v>
       </c>
       <c r="B57" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C57" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1348,10 +1363,10 @@
         <v>88</v>
       </c>
       <c r="B58" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C58" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -1359,487 +1374,519 @@
         <v>88</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="C59" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B60" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="C60" t="s">
-        <v>102</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B61" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C61" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B62" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C62" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B63" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C63" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B64" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="C64" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B65" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C65" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B66" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C66" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B67" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C67" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B68" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C68" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B69" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="C69" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B70" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C70" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B71" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C71" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B72" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="C72" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B73" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="C73" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B74" t="s">
-        <v>99</v>
+        <v>18</v>
       </c>
       <c r="C74" t="s">
-        <v>99</v>
+        <v>18</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B75" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="C75" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B76" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C76" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B77" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C77" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B78" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="C78" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B79" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="C79" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B80" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="C80" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B81" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="C81" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B82" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="C82" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B83" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="C83" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="C84" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B85" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="C85" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="C86" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C87" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="C88" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B89" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C89" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B90" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="C90" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B91" t="s">
-        <v>104</v>
+        <v>38</v>
       </c>
       <c r="C91" t="s">
-        <v>104</v>
+        <v>38</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B92" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C92" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B93" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="C93" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B94" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="C94" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B95" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="C95" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B96" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="C96" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B97" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="C97" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B98" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C98" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B99" t="s">
-        <v>9</v>
+        <v>101</v>
       </c>
       <c r="C99" t="s">
-        <v>9</v>
+        <v>101</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B100" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="C100" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B101" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="C101" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B102" t="s">
-        <v>104</v>
+        <v>34</v>
       </c>
       <c r="C102" t="s">
-        <v>104</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>87</v>
+      </c>
+      <c r="B103" t="s">
+        <v>41</v>
+      </c>
+      <c r="C103" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>87</v>
+      </c>
+      <c r="B104" t="s">
+        <v>42</v>
+      </c>
+      <c r="C104" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C99" xr:uid="{461A9C18-F1C7-4A34-90BC-0952E60C20C5}"/>
+  <autoFilter ref="A1:C104" xr:uid="{3D1B38F2-9BC7-48A6-ACF9-07AB94F89F72}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C104">
+      <sortCondition ref="A2:A104"/>
+      <sortCondition ref="B2:B104"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C104">
+    <sortCondition ref="A2:A104"/>
+    <sortCondition ref="B2:B104"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>